<commit_message>
Updated tags - removed MAN4
</commit_message>
<xml_diff>
--- a/Automatisms/Hera/pozzi_tags/Tag Pozzi con Sonde_per TLC_1.xlsx
+++ b/Automatisms/Hera/pozzi_tags/Tag Pozzi con Sonde_per TLC_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloferaudo/Desktop/Personal Data/Research activities/Unibo/Progetto_HERA_ARPAE/Automatisms/pozzi_tags/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloferaudo/Desktop/Personal Data/Research activities/Unibo/Progetto_HERA_ARPAE/Automatisms/Hera/pozzi_tags/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E48B8B-3F2D-D445-AFBF-630989F49933}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F61F76-932C-1046-BAC1-C32F92BED8B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="760" windowWidth="21480" windowHeight="13140" xr2:uid="{4B4D8BA3-11DD-45BD-9E66-A95A3732EAEC}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>TERRITORIO</t>
   </si>
@@ -130,22 +130,10 @@
     <t>BOLOGNA</t>
   </si>
   <si>
-    <t>CASTELFRANCO</t>
-  </si>
-  <si>
-    <t>B025129ABO33_1_J_LIV_FALD004_MFLIV01</t>
-  </si>
-  <si>
-    <t>B025129ABO33_1_J_POR_MISU004_MFPOR01</t>
-  </si>
-  <si>
     <t>TAG_LIV</t>
   </si>
   <si>
     <t>TAG_PORTATA</t>
-  </si>
-  <si>
-    <t>MAN4</t>
   </si>
   <si>
     <t>A5</t>
@@ -663,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED342DA-4F64-4966-8F46-0D3D9D7E0BD7}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -691,19 +679,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -714,10 +702,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -740,10 +728,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>5</v>
@@ -766,10 +754,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>6</v>
@@ -792,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>7</v>
@@ -818,7 +806,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
@@ -844,7 +832,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>13</v>
@@ -870,7 +858,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>13</v>
@@ -896,7 +884,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -922,7 +910,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>17</v>
@@ -948,7 +936,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -966,24 +954,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>24</v>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F12" s="1">
-        <v>39.5</v>
+        <v>70</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1000,13 +988,13 @@
         <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1">
         <v>70</v>
@@ -1026,13 +1014,13 @@
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F14" s="1">
         <v>70</v>
@@ -1045,51 +1033,25 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="A15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="1">
-        <v>70</v>
+      <c r="F15">
+        <v>8.8000000000000007</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="G16">
-        <v>-1</v>
-      </c>
-      <c r="H16">
         <v>0</v>
       </c>
     </row>

</xml_diff>